<commit_message>
updated url in BaseTest & testng.xml
Updated the ValidLogin to read Excel data
input.xlslx is updated with sheet ValidLogin
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B72\WorkSpace\b72framework\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\b72framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57737660-CD51-4DF4-A21F-FC90011F59B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CC3B0C-5F99-46FF-854E-BA8C16192DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5955" yWindow="4245" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>username</t>
+    <t>admin</t>
   </si>
   <si>
-    <t>admin</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>manager</t>
   </si>
 </sst>
 </file>
@@ -347,23 +353,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44681BB-C97D-4DEB-B4B6-F5F64E22853C}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>